<commit_message>
fix(mosaic_scripts.xlsx): enable cleanup job
</commit_message>
<xml_diff>
--- a/molgenis-data-model/mosaic_scripts.xlsx
+++ b/molgenis-data-model/mosaic_scripts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fkelpin/git/molgenis-app-mosaic-calculator/molgenis-data-model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612D71E1-9C58-084E-AFE9-58F5DD018FA0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C22251-3C23-AA4E-949A-CE1A2B63490A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8000" yWindow="620" windowWidth="18180" windowHeight="13320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6700" yWindow="2520" windowWidth="18180" windowHeight="13320" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sys_scr_Script" sheetId="11" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>id</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>admin</t>
-  </si>
-  <si>
-    <t>false</t>
   </si>
   <si>
     <t>0 0 0 * * ?</t>
@@ -499,7 +496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D243B1C-E38D-154F-866F-10A8D90CB792}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -542,13 +539,13 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>0</v>
@@ -562,7 +559,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>3</v>
@@ -603,7 +600,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36964475-FE3A-5045-A4C3-510469691FB1}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -621,19 +620,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>11</v>
@@ -644,19 +643,19 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="E2" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
fix(mosaic_scripts.xlsx): set extension to mosaic.pdf
</commit_message>
<xml_diff>
--- a/molgenis-data-model/mosaic_scripts.xlsx
+++ b/molgenis-data-model/mosaic_scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fkelpin/git/molgenis-app-mosaic-calculator/molgenis-data-model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01A9482-7BF0-FF46-A10C-574C9CA889E9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612D71E1-9C58-084E-AFE9-58F5DD018FA0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8000" yWindow="620" windowWidth="18180" windowHeight="13320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,9 +47,6 @@
     <t>mosaic_cleanup</t>
   </si>
   <si>
-    <t>pdf</t>
-  </si>
-  <si>
     <t>molgenis_mosaic</t>
   </si>
   <si>
@@ -111,6 +108,9 @@
   </si>
   <si>
     <t>print('Fill in contents of molgenis_cleanup.R')</t>
+  </si>
+  <si>
+    <t>mosaic.pdf</t>
   </si>
 </sst>
 </file>
@@ -500,7 +500,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -519,36 +519,36 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>0</v>
@@ -562,7 +562,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>3</v>
@@ -621,51 +621,51 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>